<commit_message>
Notules meetings, audio meeting 2
+ audio meeting 2
+- notule meeting 1
+ notule meeting 2
+- agenda meeting 1
+- agenda meeting 2
</commit_message>
<xml_diff>
--- a/documentatie/notulen/vergaderingen/notule_vergadering1.xlsx
+++ b/documentatie/notulen/vergaderingen/notule_vergadering1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Documents\GitKraken\Barroc-IT-Groep-2\documentatie\notulen\vergaderingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -160,27 +160,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Plaats: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Radius college, lokaal 320</t>
-    </r>
-  </si>
-  <si>
     <t>Vertelt wat er behandeld wordt</t>
   </si>
   <si>
@@ -308,6 +287,27 @@
   </si>
   <si>
     <t>11 Plannen volgende vergadering</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Plaats: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Radius college, lokaal 329</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -554,18 +554,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -574,6 +562,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,7 +931,7 @@
   <dimension ref="A1:Q14022"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +945,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="2"/>
@@ -968,10 +968,10 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="22"/>
       <c r="E2" s="5"/>
       <c r="F2" s="3"/>
@@ -991,10 +991,10 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="22"/>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
@@ -1014,10 +1014,10 @@
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="22"/>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
@@ -1038,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="22"/>
@@ -1087,16 +1087,16 @@
     </row>
     <row r="7" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>7</v>
@@ -1116,16 +1116,16 @@
     </row>
     <row r="8" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="26" t="s">
         <v>7</v>
@@ -1145,19 +1145,19 @@
     </row>
     <row r="9" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1174,19 +1174,19 @@
     </row>
     <row r="10" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1203,67 +1203,67 @@
     </row>
     <row r="11" spans="1:17" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>24</v>
+      <c r="D12" s="24" t="s">
+        <v>23</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>27</v>
+      <c r="E12" s="26" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="12" t="s">
+    <row r="13" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="C13" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>7</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="15" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>6</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="16" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="C16" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>6</v>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="17" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>6</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="C18" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>6</v>
@@ -1339,55 +1339,55 @@
     </row>
     <row r="19" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
@@ -43414,18 +43414,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43478,14 +43478,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F91946DA-1D0C-4852-AC5F-029A4620CB68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -43495,6 +43487,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
notule, notules update, rename map
+- notules
+ notule meeting 3
+- rename map normalisation
</commit_message>
<xml_diff>
--- a/documentatie/notulen/vergaderingen/notule_vergadering1.xlsx
+++ b/documentatie/notulen/vergaderingen/notule_vergadering1.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="30" windowWidth="20100" windowHeight="9270"/>
   </bookViews>
   <sheets>
-    <sheet name="8-9-2017" sheetId="1" r:id="rId1"/>
+    <sheet name="11-9-2017" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -43414,18 +43414,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43478,6 +43478,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F91946DA-1D0C-4852-AC5F-029A4620CB68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -43487,14 +43495,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>